<commit_message>
Added UserList test cases of ABP and modified CMCDeferredCorp in IWP
</commit_message>
<xml_diff>
--- a/KatalonData/ABPTestData/ABPTestData.xlsx
+++ b/KatalonData/ABPTestData/ABPTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\ABPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C0774511-6937-44E7-92C8-9FC9EEAD3488}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{223C1845-353A-49C9-A72C-AF1AD93DD61A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="4" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView activeTab="11" firstSheet="9" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="UIVerification-RegisterPayPage" r:id="rId1" sheetId="1"/>
@@ -19,6 +19,12 @@
     <sheet name="VerifySuccessfulPaymentPSNoCF" r:id="rId4" sheetId="4"/>
     <sheet name="VerifySuccessfulPaymentCorpNoCF" r:id="rId5" sheetId="5"/>
     <sheet name="UIVerificationPendingBillsPage" r:id="rId6" sheetId="6"/>
+    <sheet name="CreateDeleteProfileOwner" r:id="rId7" sheetId="7"/>
+    <sheet name="CreateDeletePayer" r:id="rId8" sheetId="8"/>
+    <sheet name="VerifyPasswordPolicy" r:id="rId9" sheetId="9"/>
+    <sheet name="VerifyUsernameLength" r:id="rId10" sheetId="10"/>
+    <sheet name="UiVerificationForAddUser" r:id="rId11" sheetId="11"/>
+    <sheet name="UiVerificationSPBillsLabel" r:id="rId12" sheetId="12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="69">
   <si>
     <t>BillType</t>
   </si>
@@ -179,34 +185,110 @@
     <t>Wed May 14 18:35:49 IST 2025</t>
   </si>
   <si>
-    <t>Thu May 29 19:03:27 IST 2025</t>
-  </si>
-  <si>
     <t>Available Bills Label,* Indicates required field,
 Step 1: Pay Your Bills Label(s) By Checking One or More Checkboxes in the "Check to Pay" Column Below.,One bill found.,Display,
 results,,Check to Pay,Bills Label,Due Date,Pay Date,Amount Due,Amount to Pay,Schedule to Pay,Check to Pay,ImtiazABPsingleCFBills,UDF1:*,UDF2:*,UDF3:,UDF4:,	
 1 bills selected for payment, totaling</t>
   </si>
   <si>
+    <t>Mon Jun 16 17:36:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>t476640@deluxe.com</t>
+  </si>
+  <si>
+    <t>Mon Jun 30 18:31:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Komalmis</t>
+  </si>
+  <si>
+    <t>Password must contain at least one alpha character and one numeric character.</t>
+  </si>
+  <si>
+    <t>Password must contain at least one alpha character and one numeric character.,The password must also contain at least one special character.</t>
+  </si>
+  <si>
+    <t>Komalmish@</t>
+  </si>
+  <si>
+    <t>Password must be at least 8 characters long and no more than 32 characters long.,Password must contain at least one alpha character and one numeric character.,The password must also contain at least one special character.</t>
+  </si>
+  <si>
+    <t>Mon Jun 30 20:17:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 30 20:17:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jun 30 20:18:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Username must be at least 6 characters long.</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Mon Jun 30 20:30:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Vaddahun Corp</t>
+  </si>
+  <si>
+    <t>Imtiaz</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Wed Jul 02 18:59:49 IST 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Indicates required field,
+Role: *,	
+ What's this?,
+First Name: *,	
+Last Name: *,	
+180Username: *,	
+Password: *,	
+Password must be at least 8 characters long and no more than 32 characters long. Password must contain at least one alpha character and one numeric character. The password must also contain at least one special character.,
+Confirm Password: *,
+E-mail Address: *,	
+Confirm E-mail Address: *,	
+Email Delivery Options:,Check here to receive email from this site,
+Text Receipt Phone Number:,	
+Text Delivery Options:</t>
+  </si>
+  <si>
+    <t>Tue Jul 22 16:01:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Step 1: Review bill to pay,
+Bills Label,Due Date,Date Submitted,Date Modified,Amount Due,Amount to Pay,Balance Due,
+ImtiazABPsingleCFBills,	 	 	
+UDF1:*,	
+UDF2:*,	
+UDF3:,
+UDF4:</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Thu May 29 19:06:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri May 30 16:49:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri May 30 16:51:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri May 30 16:52:15 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Jun 02 16:38:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Jun 16 17:36:34 IST 2025</t>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Thu Jul 24 18:59:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 24 19:02:30 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -249,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -292,11 +374,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
@@ -328,6 +421,21 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,6 +852,227 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="38.7265625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.7265625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" customWidth="true" width="53.36328125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="29" r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row ht="261" r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2">
+        <v>20770</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row ht="348" r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
   <dimension ref="A1:I2"/>
@@ -1113,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,13 +1479,13 @@
     </row>
     <row ht="409.5" r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1172,7 +1501,201 @@
         <v>300002</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="68.1796875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="52" r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row ht="29" r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ABP test cases and modified IWP Bootstrap deferred test cases
</commit_message>
<xml_diff>
--- a/KatalonData/ABPTestData/ABPTestData.xlsx
+++ b/KatalonData/ABPTestData/ABPTestData.xlsx
@@ -1,42 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\ABPTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476640\Documents\VPS-Katalon\KatalonData\ABPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{223C1845-353A-49C9-A72C-AF1AD93DD61A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1072E017-3256-41D3-A8C7-0480A217BEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="9" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="UIVerification-RegisterPayPage" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
-    <sheet name="SuccessfulPaymentCC" r:id="rId3" sheetId="3"/>
-    <sheet name="VerifySuccessfulPaymentPSNoCF" r:id="rId4" sheetId="4"/>
-    <sheet name="VerifySuccessfulPaymentCorpNoCF" r:id="rId5" sheetId="5"/>
-    <sheet name="UIVerificationPendingBillsPage" r:id="rId6" sheetId="6"/>
-    <sheet name="CreateDeleteProfileOwner" r:id="rId7" sheetId="7"/>
-    <sheet name="CreateDeletePayer" r:id="rId8" sheetId="8"/>
-    <sheet name="VerifyPasswordPolicy" r:id="rId9" sheetId="9"/>
-    <sheet name="VerifyUsernameLength" r:id="rId10" sheetId="10"/>
-    <sheet name="UiVerificationForAddUser" r:id="rId11" sheetId="11"/>
-    <sheet name="UiVerificationSPBillsLabel" r:id="rId12" sheetId="12"/>
+    <sheet name="UIVerification-RegisterPayPage" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="SuccessfulPaymentCC" sheetId="3" r:id="rId3"/>
+    <sheet name="VerifySuccessfulPaymentPSNoCF" sheetId="4" r:id="rId4"/>
+    <sheet name="VerifySuccessfulPaymentCorpNoCF" sheetId="5" r:id="rId5"/>
+    <sheet name="UIVerificationPendingBillsPage" sheetId="6" r:id="rId6"/>
+    <sheet name="CreateDeleteProfileOwner" sheetId="7" r:id="rId7"/>
+    <sheet name="CreateDeletePayer" sheetId="8" r:id="rId8"/>
+    <sheet name="VerifyPasswordPolicy" sheetId="9" r:id="rId9"/>
+    <sheet name="VerifyUsernameLength" sheetId="10" r:id="rId10"/>
+    <sheet name="UiVerificationForAddUser" sheetId="11" r:id="rId11"/>
+    <sheet name="UiVerificationSPBillsLabel" sheetId="12" r:id="rId12"/>
+    <sheet name="UiVerificationSPIPDaily" sheetId="13" r:id="rId13"/>
+    <sheet name="UiVerificationSPRecDeferred" sheetId="17" r:id="rId14"/>
+    <sheet name="UiVerificationSPRecDaily" sheetId="19" r:id="rId15"/>
+    <sheet name="UiVerificationSPAP" sheetId="18" r:id="rId16"/>
+    <sheet name="UiVerificationSPInstallmentQuar" sheetId="14" r:id="rId17"/>
+    <sheet name="UiVerificationSPInstallmentAnua" sheetId="15" r:id="rId18"/>
+    <sheet name="UiVerificationSPIPDeferred" sheetId="16" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="84">
   <si>
     <t>BillType</t>
   </si>
@@ -191,9 +210,6 @@
 1 bills selected for payment, totaling</t>
   </si>
   <si>
-    <t>Mon Jun 16 17:36:34 IST 2025</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -279,9 +295,6 @@
 UDF4:</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -289,13 +302,106 @@
   </si>
   <si>
     <t>Thu Jul 24 19:02:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 13 12:44:44 IST 2025</t>
+  </si>
+  <si>
+    <t>VTList1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Payment Plan Frequency,
+Quarterly,
+Select the date you wish to submit your first payment and it will recur every three months on that day,
+Note: Any payments associated with the payment plan that are scheduled on a date that does not exist (eg. February 30th, April 31st), will be processed on the first day of the following month.,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into, 
+Individual Amount:,	Repeat this amount until the Balance Due is achieved: $ ,
+Step 4: Review Payment Plan
+1 Quarterly payment of $10.00 on </t>
+  </si>
+  <si>
+    <t>Wed Aug 13 22:22:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Select Payment Plan Frequency,
+Annual,
+Select the date you wish to submit your first payment and it will recur every year on that day,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into,
+Individual Amount:,Repeat this amount until the Balance Due is achieved: $</t>
+  </si>
+  <si>
+    <t>ReviewConvinienceFee</t>
+  </si>
+  <si>
+    <t>CFAmount</t>
+  </si>
+  <si>
+    <t>Wed Sep 03 02:50:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Select Payment Plan Frequency,
+Daily,
+Select the date you wish to submit your first payment and it will recur every day after,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into ,
+Individual Amount:,Repeat this amount until the Balance Due is achieved: $, 
+Step 4: Review Payment Plan,
+1 Daily payment of $</t>
+  </si>
+  <si>
+    <t>Wed Sep 03 14:31:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Select the date you wish to submit your payment,Divide your payment plan by...,
+ Number of Payments:,	Divide the Balance Due into 
+,payments,
+ Individual Amount:,	Repeat this amount until the Balance Due is achieved: $, 
+10.00,
+Step 4: Review Payment Plan,
+1 Deferred payment of $</t>
+  </si>
+  <si>
+    <t>Select Payment Plan Frequency,
+Deferred,
+Select the date you wish to submit your payment,
+Step 4: Review Payment Plan,
+1 Deferred payment of $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 4: Review Payment Plan,
+Amount due will be paid 3 calendar days before the Due Date,
+Step 5: Review Your Convenience Fees,
+Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:	</t>
+  </si>
+  <si>
+    <t>Wed Sep 03 19:41:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 03 20:03:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Recurring Fixed Amount Payment - The same amount is paid at a determined frequency.,
+ Automatic Payment - Bills are automatically paid 3 calendar days before the Due Date.,Select Payment Plan Frequency,
+Daily,
+Select the date you wish to submit your first payment and it will recur every day after,
+Step 4: Review Payment Plan,
+Daily payments of $</t>
+  </si>
+  <si>
+    <t>Wed Sep 03 20:10:40 IST 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,62 +493,68 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -459,10 +571,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -497,7 +609,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -532,7 +644,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -626,21 +738,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -657,7 +769,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -709,15 +821,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:I2"/>
@@ -725,12 +837,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="8" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.6328125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.6328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -783,7 +895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row ht="409.5" r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
@@ -845,7 +957,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -853,8 +965,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G2"/>
@@ -862,9 +974,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="38.7265625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="38.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -881,13 +993,13 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>56</v>
+      <c r="G1" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -895,30 +1007,30 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:G2"/>
@@ -926,10 +1038,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="53.36328125" collapsed="true"/>
+    <col min="6" max="6" width="53.36328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -943,63 +1055,63 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row ht="261" r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="261" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="L2" t="s">
@@ -1010,21 +1122,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1038,44 +1150,636 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row ht="348" r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G1" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="348" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>64</v>
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED305E-1D1F-4473-A9FE-10CCE4EF2A93}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="34.36328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="15" t="str">
+        <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
+        <v>09/05/2025</v>
+      </c>
+      <c r="H2" s="18">
+        <v>10</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16" t="str">
+        <f ca="1">F2&amp;TEXT(H2,"0.00")&amp;" on "&amp;G2&amp;","&amp;K2</f>
+        <v>Select Payment Plan Frequency,
+Daily,
+Select the date you wish to submit your first payment and it will recur every day after,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into ,
+Individual Amount:,Repeat this amount until the Balance Due is achieved: $, 
+Step 4: Review Payment Plan,
+1 Daily payment of $10.00 on 09/05/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 0.00 starting on 09/05/2025</v>
+      </c>
+      <c r="K2" s="14" t="str">
+        <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Daily payment of "&amp;  TEXT(I2,"0.00")&amp;" starting on "&amp;G2</f>
+        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 0.00 starting on 09/05/2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4382B992-23F5-4C47-8E0D-617770DAB873}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="27.6328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.36328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.7265625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="15" t="str">
+        <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
+        <v>09/05/2025</v>
+      </c>
+      <c r="H2" s="18">
+        <v>10</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16" t="str">
+        <f ca="1">F2&amp;TEXT(H2,"0.00")&amp;" on "&amp;G2&amp;","&amp;K2</f>
+        <v>Select Payment Plan Frequency,
+Deferred,
+Select the date you wish to submit your payment,
+Step 4: Review Payment Plan,
+1 Deferred payment of $10.00 on 09/05/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:</v>
+      </c>
+      <c r="K2" s="14" t="str">
+        <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Deferred payment of "&amp;  TEXT(I2,"0.00")&amp;" starting on "&amp;G2&amp;" ,Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:"</f>
+        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EA3BF1-14B8-47AF-A2C8-3C7ED7468772}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="29.90625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.453125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.7265625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="15" t="str">
+        <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
+        <v>09/05/2025</v>
+      </c>
+      <c r="H2" s="18">
+        <v>10</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16" t="str">
+        <f ca="1">F2&amp;TEXT(H2,"0.00")&amp;" starting on "&amp;G2&amp;","&amp;K2</f>
+        <v>Recurring Fixed Amount Payment - The same amount is paid at a determined frequency.,
+ Automatic Payment - Bills are automatically paid 3 calendar days before the Due Date.,Select Payment Plan Frequency,
+Daily,
+Select the date you wish to submit your first payment and it will recur every day after,
+Step 4: Review Payment Plan,
+Daily payments of $10.00 starting on 09/05/2025,A Convenience Fee will be added to each transaction issued for Daily payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:</v>
+      </c>
+      <c r="K2" s="14" t="str">
+        <f ca="1">"A Convenience Fee will be added to each transaction issued for Daily payment of "&amp;  TEXT(I2,"0.00")&amp;" starting on "&amp;G2&amp;" ,Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:"</f>
+        <v>A Convenience Fee will be added to each transaction issued for Daily payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+Total Convenience Fees Paid:,	
+Total Paid under this plan:</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59FD46A-A4BF-4EFF-8C85-302E7420C761}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="40.54296875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D81D62B-D7FF-4418-A543-2CCEB8B27904}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="39.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="14" t="str">
+        <f ca="1">F2&amp;TEXT(TODAY()+1,"mm/dd/yyyy")</f>
+        <v>Select Payment Plan Frequency,
+Quarterly,
+Select the date you wish to submit your first payment and it will recur every three months on that day,
+Note: Any payments associated with the payment plan that are scheduled on a date that does not exist (eg. February 30th, April 31st), will be processed on the first day of the following month.,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into, 
+Individual Amount:,	Repeat this amount until the Balance Due is achieved: $ ,
+Step 4: Review Payment Plan
+1 Quarterly payment of $10.00 on 09/05/2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6951466-0A68-4F4C-8CFE-91C88774BAFD}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="32.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="319" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="16" t="str">
+        <f ca="1">F2&amp;TEXT(TODAY()+1,"mm/dd/yyyy")</f>
+        <v>Select Payment Plan Frequency,
+Annual,
+Select the date you wish to submit your first payment and it will recur every year on that day,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into,
+Individual Amount:,Repeat this amount until the Balance Due is achieved: $09/05/2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106EA5F4-3A74-4B88-9694-190DD754DB42}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="35.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.54296875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="31.26953125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="232" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="15" t="str">
+        <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
+        <v>09/04/2025</v>
+      </c>
+      <c r="G2" s="18">
+        <v>10</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="16" t="str">
+        <f ca="1">E2&amp;TEXT(G2,"0.00")&amp;" on "&amp;F2&amp;","&amp;J2</f>
+        <v>Select the date you wish to submit your payment,Divide your payment plan by...,
+ Number of Payments:,	Divide the Balance Due into 
+,payments,
+ Individual Amount:,	Repeat this amount until the Balance Due is achieved: $, 
+10.00,
+Step 4: Review Payment Plan,
+1 Deferred payment of $10.00 on 09/04/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/04/2025</v>
+      </c>
+      <c r="J2" s="14" t="str">
+        <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Deferred payment of "&amp;  TEXT(H2,"0.00")&amp;" starting on "&amp;F2</f>
+        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/04/2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H2"/>
@@ -1083,8 +1787,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.08984375" collapsed="true"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1137,13 +1841,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCBBA-7D6F-4A96-ABDF-B9688B9AD57A}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCBBA-7D6F-4A96-ABDF-B9688B9AD57A}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -1151,9 +1855,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.90625" collapsed="true"/>
+    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1277,13 +1981,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E036A-EB5C-429E-B5B6-2CEB663A49DE}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E036A-EB5C-429E-B5B6-2CEB663A49DE}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J2"/>
@@ -1291,10 +1995,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1357,13 +2061,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8A1DA2-5F25-403C-A696-AD0A990EA2A5}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8A1DA2-5F25-403C-A696-AD0A990EA2A5}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -1371,7 +2075,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1434,13 +2138,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -1477,15 +2181,15 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="409.5" r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1505,13 +2209,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -1519,7 +2223,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1536,7 +2240,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1544,24 +2248,24 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -1583,7 +2287,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1591,24 +2295,24 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -1616,8 +2320,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="68.1796875" collapsed="true"/>
+    <col min="5" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="68.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1634,51 +2338,51 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="52" r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row ht="29" r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1686,19 +2390,19 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Object repository for Pay As a guest page and ABp test suite
</commit_message>
<xml_diff>
--- a/KatalonData/ABPTestData/ABPTestData.xlsx
+++ b/KatalonData/ABPTestData/ABPTestData.xlsx
@@ -1,42 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476640\Documents\VPS-Katalon\KatalonData\ABPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1072E017-3256-41D3-A8C7-0480A217BEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1072E017-3256-41D3-A8C7-0480A217BEDF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="14" firstSheet="12" windowHeight="10300" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="UIVerification-RegisterPayPage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="SuccessfulPaymentCC" sheetId="3" r:id="rId3"/>
-    <sheet name="VerifySuccessfulPaymentPSNoCF" sheetId="4" r:id="rId4"/>
-    <sheet name="VerifySuccessfulPaymentCorpNoCF" sheetId="5" r:id="rId5"/>
-    <sheet name="UIVerificationPendingBillsPage" sheetId="6" r:id="rId6"/>
-    <sheet name="CreateDeleteProfileOwner" sheetId="7" r:id="rId7"/>
-    <sheet name="CreateDeletePayer" sheetId="8" r:id="rId8"/>
-    <sheet name="VerifyPasswordPolicy" sheetId="9" r:id="rId9"/>
-    <sheet name="VerifyUsernameLength" sheetId="10" r:id="rId10"/>
-    <sheet name="UiVerificationForAddUser" sheetId="11" r:id="rId11"/>
-    <sheet name="UiVerificationSPBillsLabel" sheetId="12" r:id="rId12"/>
-    <sheet name="UiVerificationSPIPDaily" sheetId="13" r:id="rId13"/>
-    <sheet name="UiVerificationSPRecDeferred" sheetId="17" r:id="rId14"/>
-    <sheet name="UiVerificationSPRecDaily" sheetId="19" r:id="rId15"/>
-    <sheet name="UiVerificationSPAP" sheetId="18" r:id="rId16"/>
-    <sheet name="UiVerificationSPInstallmentQuar" sheetId="14" r:id="rId17"/>
-    <sheet name="UiVerificationSPInstallmentAnua" sheetId="15" r:id="rId18"/>
-    <sheet name="UiVerificationSPIPDeferred" sheetId="16" r:id="rId19"/>
+    <sheet name="UIVerification-RegisterPayPage" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
+    <sheet name="SuccessfulPaymentCC" r:id="rId3" sheetId="3"/>
+    <sheet name="VerifySuccessfulPaymentPSNoCF" r:id="rId4" sheetId="4"/>
+    <sheet name="VerifySuccessfulPaymentCorpNoCF" r:id="rId5" sheetId="5"/>
+    <sheet name="UIVerificationPendingBillsPage" r:id="rId6" sheetId="6"/>
+    <sheet name="CreateDeleteProfileOwner" r:id="rId7" sheetId="7"/>
+    <sheet name="CreateDeletePayer" r:id="rId8" sheetId="8"/>
+    <sheet name="VerifyPasswordPolicy" r:id="rId9" sheetId="9"/>
+    <sheet name="VerifyUsernameLength" r:id="rId10" sheetId="10"/>
+    <sheet name="UiVerificationForAddUser" r:id="rId11" sheetId="11"/>
+    <sheet name="UiVerificationSPBillsLabel" r:id="rId12" sheetId="12"/>
+    <sheet name="UiVerificationSPIPDaily" r:id="rId13" sheetId="13"/>
+    <sheet name="UiVerificationSPRecDeferred" r:id="rId14" sheetId="17"/>
+    <sheet name="UiVerificationSPRecDaily" r:id="rId15" sheetId="19"/>
+    <sheet name="UiVerificationSPAP" r:id="rId16" sheetId="18"/>
+    <sheet name="UiVerificationSPInstallmentQuar" r:id="rId17" sheetId="14"/>
+    <sheet name="UiVerificationSPInstallmentAnua" r:id="rId18" sheetId="15"/>
+    <sheet name="UiVerificationSPIPDeferred" r:id="rId19" sheetId="16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="135">
   <si>
     <t>BillType</t>
   </si>
@@ -393,6 +393,159 @@
   </si>
   <si>
     <t>Wed Sep 03 20:10:40 IST 2025</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:45:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:46:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:46:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:47:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:48:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:48:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:49:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:50:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:50:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:53:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:54:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:54:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:55:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:57:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:57:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:58:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Sep 19 21:58:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:19:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:20:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:20:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:22:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:22:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:23:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:23:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:24:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:25:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:28:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:28:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:29:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:30:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:31:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:32:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:32:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Sep 24 17:33:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:00:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:00:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:01:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:02:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:03:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:04:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:04:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:05:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:08:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:09:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:09:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:10:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:12:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:12:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:13:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 25 14:13:52 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -493,68 +646,68 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -571,10 +724,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -609,7 +762,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -644,7 +797,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -738,21 +891,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -769,7 +922,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -821,15 +974,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:I2"/>
@@ -837,12 +990,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.6328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="6" max="8" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.6328125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -895,7 +1048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.35">
+    <row ht="409.5" r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
@@ -957,7 +1110,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -965,8 +1118,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G2"/>
@@ -974,9 +1127,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="38.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="38.7265625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1007,7 +1160,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1024,13 +1177,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:G2"/>
@@ -1038,10 +1191,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="53.36328125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="53.36328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1082,12 +1235,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="261" x14ac:dyDescent="0.35">
+    <row ht="261" r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1122,13 +1275,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
@@ -1136,7 +1289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1159,12 +1312,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="348" x14ac:dyDescent="0.35">
+    <row ht="348" r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1181,13 +1334,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED305E-1D1F-4473-A9FE-10CCE4EF2A93}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED305E-1D1F-4473-A9FE-10CCE4EF2A93}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -1195,12 +1348,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="34.36328125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="34.36328125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row ht="43.5" r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1235,12 +1388,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="362.5" x14ac:dyDescent="0.35">
+    <row ht="362.5" r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1279,13 +1432,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4382B992-23F5-4C47-8E0D-617770DAB873}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4382B992-23F5-4C47-8E0D-617770DAB873}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -1293,12 +1446,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="27.6328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.36328125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.7265625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="27.6328125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.36328125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1333,12 +1486,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
+    <row ht="304.5" r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1380,13 +1533,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EA3BF1-14B8-47AF-A2C8-3C7ED7468772}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EA3BF1-14B8-47AF-A2C8-3C7ED7468772}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
@@ -1394,12 +1547,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="29.90625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.7265625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="29.90625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="29.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1434,12 +1587,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
+    <row ht="304.5" r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1482,13 +1635,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59FD46A-A4BF-4EFF-8C85-302E7420C761}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59FD46A-A4BF-4EFF-8C85-302E7420C761}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -1496,7 +1649,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="40.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="40.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1519,12 +1672,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+    <row ht="101.5" r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1538,13 +1691,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D81D62B-D7FF-4418-A543-2CCEB8B27904}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D81D62B-D7FF-4418-A543-2CCEB8B27904}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -1552,8 +1705,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="39.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.1796875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="39.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1579,12 +1732,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
+    <row ht="246.5" r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1610,13 +1763,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6951466-0A68-4F4C-8CFE-91C88774BAFD}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6951466-0A68-4F4C-8CFE-91C88774BAFD}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G2"/>
@@ -1624,8 +1777,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="32.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="32.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1651,12 +1804,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="319" x14ac:dyDescent="0.35">
+    <row ht="319" r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1679,13 +1832,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106EA5F4-3A74-4B88-9694-190DD754DB42}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106EA5F4-3A74-4B88-9694-190DD754DB42}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1693,15 +1846,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="35.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.54296875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="29.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="31.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="35.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.54296875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="31.26953125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1733,12 +1886,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="232" x14ac:dyDescent="0.35">
+    <row ht="232" r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1773,13 +1926,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H2"/>
@@ -1787,8 +1940,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.08984375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1841,13 +1994,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCBBA-7D6F-4A96-ABDF-B9688B9AD57A}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCBBA-7D6F-4A96-ABDF-B9688B9AD57A}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -1855,9 +2008,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.90625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1981,13 +2134,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E036A-EB5C-429E-B5B6-2CEB663A49DE}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E036A-EB5C-429E-B5B6-2CEB663A49DE}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J2"/>
@@ -1995,10 +2148,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2061,13 +2214,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8A1DA2-5F25-403C-A696-AD0A990EA2A5}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8A1DA2-5F25-403C-A696-AD0A990EA2A5}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -2075,7 +2228,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2138,13 +2291,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -2181,12 +2334,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+    <row ht="409.5" r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2209,13 +2362,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -2223,7 +2376,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2248,7 +2401,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2259,13 +2412,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -2295,7 +2448,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2306,13 +2459,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -2320,8 +2473,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="68.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="68.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2347,12 +2500,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row customHeight="1" ht="52" r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2368,12 +2521,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -2390,7 +2543,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -2403,6 +2556,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated test cases which were failing
</commit_message>
<xml_diff>
--- a/KatalonData/ABPTestData/ABPTestData.xlsx
+++ b/KatalonData/ABPTestData/ABPTestData.xlsx
@@ -1,42 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476640\Documents\VPS-Katalon\KatalonData\ABPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{1072E017-3256-41D3-A8C7-0480A217BEDF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8350BB-EB28-4064-9AA7-065E84252D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="14" firstSheet="12" windowHeight="10300" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="17" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="UIVerification-RegisterPayPage" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
-    <sheet name="SuccessfulPaymentCC" r:id="rId3" sheetId="3"/>
-    <sheet name="VerifySuccessfulPaymentPSNoCF" r:id="rId4" sheetId="4"/>
-    <sheet name="VerifySuccessfulPaymentCorpNoCF" r:id="rId5" sheetId="5"/>
-    <sheet name="UIVerificationPendingBillsPage" r:id="rId6" sheetId="6"/>
-    <sheet name="CreateDeleteProfileOwner" r:id="rId7" sheetId="7"/>
-    <sheet name="CreateDeletePayer" r:id="rId8" sheetId="8"/>
-    <sheet name="VerifyPasswordPolicy" r:id="rId9" sheetId="9"/>
-    <sheet name="VerifyUsernameLength" r:id="rId10" sheetId="10"/>
-    <sheet name="UiVerificationForAddUser" r:id="rId11" sheetId="11"/>
-    <sheet name="UiVerificationSPBillsLabel" r:id="rId12" sheetId="12"/>
-    <sheet name="UiVerificationSPIPDaily" r:id="rId13" sheetId="13"/>
-    <sheet name="UiVerificationSPRecDeferred" r:id="rId14" sheetId="17"/>
-    <sheet name="UiVerificationSPRecDaily" r:id="rId15" sheetId="19"/>
-    <sheet name="UiVerificationSPAP" r:id="rId16" sheetId="18"/>
-    <sheet name="UiVerificationSPInstallmentQuar" r:id="rId17" sheetId="14"/>
-    <sheet name="UiVerificationSPInstallmentAnua" r:id="rId18" sheetId="15"/>
-    <sheet name="UiVerificationSPIPDeferred" r:id="rId19" sheetId="16"/>
+    <sheet name="UIVerification-RegisterPayPage" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="SuccessfulPaymentCC" sheetId="3" r:id="rId3"/>
+    <sheet name="VerifySuccessfulPaymentPSNoCF" sheetId="4" r:id="rId4"/>
+    <sheet name="VerifySuccessfulPaymentCorpNoCF" sheetId="5" r:id="rId5"/>
+    <sheet name="UIVerificationPendingBillsPage" sheetId="6" r:id="rId6"/>
+    <sheet name="CreateDeleteProfileOwner" sheetId="7" r:id="rId7"/>
+    <sheet name="CreateDeletePayer" sheetId="8" r:id="rId8"/>
+    <sheet name="VerifyPasswordPolicy" sheetId="9" r:id="rId9"/>
+    <sheet name="VerifyUsernameLength" sheetId="10" r:id="rId10"/>
+    <sheet name="UiVerificationForAddUser" sheetId="11" r:id="rId11"/>
+    <sheet name="UiVerificationForAccountProfile" sheetId="20" r:id="rId12"/>
+    <sheet name="UiVerificationSPBillsLabel" sheetId="12" r:id="rId13"/>
+    <sheet name="UiVerificationSPIPDaily" sheetId="13" r:id="rId14"/>
+    <sheet name="UiVerificationSPRecDeferred" sheetId="17" r:id="rId15"/>
+    <sheet name="UiVerificationSPRecDaily" sheetId="19" r:id="rId16"/>
+    <sheet name="UiVerificationSPAP" sheetId="18" r:id="rId17"/>
+    <sheet name="UiVerificationSPInstallmentQuar" sheetId="14" r:id="rId18"/>
+    <sheet name="UiVerificationSPInstallmentAnua" sheetId="15" r:id="rId19"/>
+    <sheet name="UiVerificationSPIPDeferred" sheetId="16" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="86">
   <si>
     <t>BillType</t>
   </si>
@@ -216,9 +216,6 @@
     <t>t476640@deluxe.com</t>
   </si>
   <si>
-    <t>Mon Jun 30 18:31:22 IST 2025</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -237,24 +234,12 @@
     <t>Password must be at least 8 characters long and no more than 32 characters long.,Password must contain at least one alpha character and one numeric character.,The password must also contain at least one special character.</t>
   </si>
   <si>
-    <t>Mon Jun 30 20:17:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Jun 30 20:17:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Mon Jun 30 20:18:07 IST 2025</t>
-  </si>
-  <si>
     <t>Username must be at least 6 characters long.</t>
   </si>
   <si>
     <t>UserName</t>
   </si>
   <si>
-    <t>Mon Jun 30 20:30:37 IST 2025</t>
-  </si>
-  <si>
     <t>Vaddahun Corp</t>
   </si>
   <si>
@@ -262,9 +247,6 @@
   </si>
   <si>
     <t>Ahmed</t>
-  </si>
-  <si>
-    <t>Wed Jul 02 18:59:49 IST 2025</t>
   </si>
   <si>
     <t xml:space="preserve"> * Indicates required field,
@@ -283,28 +265,7 @@
 Text Delivery Options:</t>
   </si>
   <si>
-    <t>Tue Jul 22 16:01:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Step 1: Review bill to pay,
-Bills Label,Due Date,Date Submitted,Date Modified,Amount Due,Amount to Pay,Balance Due,
-ImtiazABPsingleCFBills,	 	 	
-UDF1:*,	
-UDF2:*,	
-UDF3:,
-UDF4:</t>
-  </si>
-  <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>Thu Jul 24 18:59:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Jul 24 19:02:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Aug 13 12:44:44 IST 2025</t>
   </si>
   <si>
     <t>VTList1</t>
@@ -321,24 +282,10 @@
 1 Quarterly payment of $10.00 on </t>
   </si>
   <si>
-    <t>Wed Aug 13 22:22:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Select Payment Plan Frequency,
-Annual,
-Select the date you wish to submit your first payment and it will recur every year on that day,
-Divide your payment plan by...,
-Number of Payments:,Divide the Balance Due into,
-Individual Amount:,Repeat this amount until the Balance Due is achieved: $</t>
-  </si>
-  <si>
     <t>ReviewConvinienceFee</t>
   </si>
   <si>
     <t>CFAmount</t>
-  </si>
-  <si>
-    <t>Wed Sep 03 02:50:43 IST 2025</t>
   </si>
   <si>
     <t>Select Payment Plan Frequency,
@@ -351,9 +298,6 @@
 1 Daily payment of $</t>
   </si>
   <si>
-    <t>Wed Sep 03 14:31:07 IST 2025</t>
-  </si>
-  <si>
     <t>Select the date you wish to submit your payment,Divide your payment plan by...,
  Number of Payments:,	Divide the Balance Due into 
 ,payments,
@@ -378,12 +322,6 @@
 Total Paid under this plan:	</t>
   </si>
   <si>
-    <t>Wed Sep 03 19:41:47 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 03 20:03:53 IST 2025</t>
-  </si>
-  <si>
     <t>Recurring Fixed Amount Payment - The same amount is paid at a determined frequency.,
  Automatic Payment - Bills are automatically paid 3 calendar days before the Due Date.,Select Payment Plan Frequency,
 Daily,
@@ -392,160 +330,85 @@
 Daily payments of $</t>
   </si>
   <si>
-    <t>Wed Sep 03 20:10:40 IST 2025</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:45:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:46:04 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:46:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:47:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:48:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:48:58 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:49:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:50:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:50:55 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:53:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:54:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:54:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:55:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:57:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:57:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:58:09 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Sep 19 21:58:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:19:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:20:00 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:20:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:22:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:22:49 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:23:13 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:23:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:24:39 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:25:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:28:07 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:28:48 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:29:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:30:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:31:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:32:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:32:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Sep 24 17:33:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:00:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:00:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:01:13 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:02:44 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:03:41 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:04:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:04:58 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:05:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:08:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:09:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:09:47 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:10:39 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:12:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:12:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:13:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Sep 25 14:13:52 IST 2025</t>
+    <t>Tue Oct 14 17:27:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:28:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:30:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:30:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:31:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:34:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:35:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:36:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:37:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:38:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:38:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 17:39:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Oct 14 23:27:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 00:51:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Account Profile,
+* Indicates required field,
+Company Name:,	
+First Name:,	
+Last Name:,	
+Address Line 1: *,	
+Address Line 2: ,  	
+Country: *,	
+ZIP: *,	
+City: *	,
+State : *,</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 00:59:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Step 1: Review bill to pay,
+Bills Label,Due Date,Date Submitted,Date Modified,Amount Due,Amount to Pay,Balance Due,
+ImtiazABPdoubleCFBills ,	 	 	
+UDF1:*,	
+UDF2:,	
+UDF3:,
+UDF4:*</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 01:18:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 01:20:09 IST 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Payment Plan Frequency,
+Annual,
+Select the date you wish to submit your first payment and it will recur every year on that day,
+Divide your payment plan by...,
+Number of Payments:,Divide the Balance Due into,
+Individual Amount:,Repeat this amount until the Balance Due is achieved: $,1 Annual payment of $10.00 on </t>
   </si>
 </sst>
 </file>
@@ -646,68 +509,68 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -724,10 +587,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -762,7 +625,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -797,7 +660,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -891,21 +754,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -922,7 +785,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -974,15 +837,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:I2"/>
@@ -990,12 +853,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="8" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.6328125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.90625" collapsed="true"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.6328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -1048,7 +911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row ht="409.5" r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
@@ -1110,7 +973,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1118,8 +981,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409B366-E307-4873-AD1A-14C5ECF78921}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G2"/>
@@ -1127,9 +990,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="38.7265625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="38.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1152,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1160,7 +1023,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1170,31 +1033,31 @@
         <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DFE7B9-88F3-4E87-BB56-955EB38799F0}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="53.36328125" collapsed="true"/>
+    <col min="6" max="6" width="53.36328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +1077,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
@@ -1235,12 +1098,12 @@
         <v>18</v>
       </c>
     </row>
-    <row ht="261" r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="261" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1250,19 +1113,19 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>23</v>
@@ -1275,21 +1138,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EBD9BD-D9A5-41D7-B0D1-A7DD8841A698}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="39.7265625" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1309,15 +1175,33 @@
         <v>10</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row ht="348" r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1327,20 +1211,100 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
+      <c r="H2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2">
+        <v>20770</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED305E-1D1F-4473-A9FE-10CCE4EF2A93}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5A32-AE5F-4469-909E-B5CBB0B316F1}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="44.26953125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED305E-1D1F-4473-A9FE-10CCE4EF2A93}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -1348,12 +1312,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="34.36328125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" width="34.36328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="43.5" r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1370,7 +1334,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>5</v>
@@ -1379,21 +1343,21 @@
         <v>25</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row ht="362.5" r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1403,11 +1367,11 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G2" s="15" t="str">
         <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
-        <v>09/05/2025</v>
+        <v>10/16/2025</v>
       </c>
       <c r="H2" s="18">
         <v>10</v>
@@ -1424,21 +1388,21 @@
 Number of Payments:,Divide the Balance Due into ,
 Individual Amount:,Repeat this amount until the Balance Due is achieved: $, 
 Step 4: Review Payment Plan,
-1 Daily payment of $10.00 on 09/05/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 0.00 starting on 09/05/2025</v>
+1 Daily payment of $10.00 on 10/16/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 0.00 starting on 10/16/2025</v>
       </c>
       <c r="K2" s="14" t="str">
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Daily payment of "&amp;  TEXT(I2,"0.00")&amp;" starting on "&amp;G2</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 0.00 starting on 09/05/2025</v>
+        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 0.00 starting on 10/16/2025</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4382B992-23F5-4C47-8E0D-617770DAB873}">
-  <dimension ref="A1:L2"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4382B992-23F5-4C47-8E0D-617770DAB873}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -1446,12 +1410,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="27.6328125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.36328125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.7265625" collapsed="true"/>
+    <col min="6" max="6" width="27.6328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.36328125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1432,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>5</v>
@@ -1477,21 +1441,21 @@
         <v>25</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row ht="304.5" r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1501,11 +1465,11 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="G2" s="15" t="str">
         <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
-        <v>09/05/2025</v>
+        <v>10/16/2025</v>
       </c>
       <c r="H2" s="18">
         <v>10</v>
@@ -1519,7 +1483,7 @@
 Deferred,
 Select the date you wish to submit your payment,
 Step 4: Review Payment Plan,
-1 Deferred payment of $10.00 on 09/05/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+1 Deferred payment of $10.00 on 10/16/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 10/16/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -1527,32 +1491,32 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Deferred payment of "&amp;  TEXT(I2,"0.00")&amp;" starting on "&amp;G2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 10/16/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EA3BF1-14B8-47AF-A2C8-3C7ED7468772}">
-  <dimension ref="A1:L2"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EA3BF1-14B8-47AF-A2C8-3C7ED7468772}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="29.90625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="29.453125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.7265625" collapsed="true"/>
+    <col min="6" max="6" width="29.90625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.453125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1569,7 +1533,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>5</v>
@@ -1578,21 +1542,21 @@
         <v>25</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row ht="304.5" r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1602,11 +1566,11 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G2" s="15" t="str">
         <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
-        <v>09/05/2025</v>
+        <v>10/16/2025</v>
       </c>
       <c r="H2" s="18">
         <v>10</v>
@@ -1621,7 +1585,7 @@
 Daily,
 Select the date you wish to submit your first payment and it will recur every day after,
 Step 4: Review Payment Plan,
-Daily payments of $10.00 starting on 09/05/2025,A Convenience Fee will be added to each transaction issued for Daily payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+Daily payments of $10.00 starting on 10/16/2025,A Convenience Fee will be added to each transaction issued for Daily payment of 0.00 starting on 10/16/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -1629,19 +1593,19 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for Daily payment of "&amp;  TEXT(I2,"0.00")&amp;" starting on "&amp;G2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for Daily payment of 0.00 starting on 09/05/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for Daily payment of 0.00 starting on 10/16/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59FD46A-A4BF-4EFF-8C85-302E7420C761}">
-  <dimension ref="A1:G2"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59FD46A-A4BF-4EFF-8C85-302E7420C761}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -1649,7 +1613,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="40.54296875" collapsed="true"/>
+    <col min="6" max="6" width="40.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1672,12 +1636,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="101.5" r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1687,17 +1651,17 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D81D62B-D7FF-4418-A543-2CCEB8B27904}">
-  <dimension ref="A1:H2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D81D62B-D7FF-4418-A543-2CCEB8B27904}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -1705,8 +1669,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="39.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.1796875" collapsed="true"/>
+    <col min="6" max="6" width="39.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1726,18 +1690,18 @@
         <v>42</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row ht="246.5" r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1747,7 +1711,7 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G2" s="14" t="str">
         <f ca="1">F2&amp;TEXT(TODAY()+1,"mm/dd/yyyy")</f>
@@ -1759,26 +1723,26 @@
 Number of Payments:,Divide the Balance Due into, 
 Individual Amount:,	Repeat this amount until the Balance Due is achieved: $ ,
 Step 4: Review Payment Plan
-1 Quarterly payment of $10.00 on 09/05/2025</v>
+1 Quarterly payment of $10.00 on 10/16/2025</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6951466-0A68-4F4C-8CFE-91C88774BAFD}">
-  <dimension ref="A1:H2"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6951466-0A68-4F4C-8CFE-91C88774BAFD}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="32.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="6" max="6" width="53.6328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1798,18 +1762,18 @@
         <v>42</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row ht="319" r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -1819,7 +1783,7 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="G2" s="16" t="str">
         <f ca="1">F2&amp;TEXT(TODAY()+1,"mm/dd/yyyy")</f>
@@ -1828,17 +1792,85 @@
 Select the date you wish to submit your first payment and it will recur every year on that day,
 Divide your payment plan by...,
 Number of Payments:,Divide the Balance Due into,
-Individual Amount:,Repeat this amount until the Balance Due is achieved: $09/05/2025</v>
+Individual Amount:,Repeat this amount until the Balance Due is achieved: $,1 Annual payment of $10.00 on 10/16/2025</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106EA5F4-3A74-4B88-9694-190DD754DB42}">
-  <dimension ref="A1:K2"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.08984375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106EA5F4-3A74-4B88-9694-190DD754DB42}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1846,15 +1878,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="35.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.54296875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="7.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="29.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="5" max="5" width="35.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.54296875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="31.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +1900,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>5</v>
@@ -1877,32 +1909,32 @@
         <v>25</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row ht="232" r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="232" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F2" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>09/04/2025</v>
+        <v>10/15/2025</v>
       </c>
       <c r="G2" s="18">
         <v>10</v>
@@ -1918,89 +1950,21 @@
  Individual Amount:,	Repeat this amount until the Balance Due is achieved: $, 
 10.00,
 Step 4: Review Payment Plan,
-1 Deferred payment of $10.00 on 09/04/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/04/2025</v>
+1 Deferred payment of $10.00 on 10/15/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 10/15/2025</v>
       </c>
       <c r="J2" s="14" t="str">
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Deferred payment of "&amp;  TEXT(H2,"0.00")&amp;" starting on "&amp;F2</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 09/04/2025</v>
+        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 0.00 starting on 10/15/2025</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59C5AD-9583-4572-BF59-08E264185AA4}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.08984375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCBBA-7D6F-4A96-ABDF-B9688B9AD57A}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22FCBBA-7D6F-4A96-ABDF-B9688B9AD57A}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K2"/>
@@ -2008,9 +1972,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.90625" collapsed="true"/>
+    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2134,13 +2098,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E036A-EB5C-429E-B5B6-2CEB663A49DE}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E036A-EB5C-429E-B5B6-2CEB663A49DE}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J2"/>
@@ -2148,10 +2112,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2214,13 +2178,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8A1DA2-5F25-403C-A696-AD0A990EA2A5}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8A1DA2-5F25-403C-A696-AD0A990EA2A5}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -2228,7 +2192,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2291,13 +2255,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3003305-5779-4E10-BB96-1E05DA55CF7C}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -2334,12 +2298,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="409.5" r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2362,13 +2326,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8EB073-2CB6-4360-AD8F-5A1F832738F2}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -2376,7 +2340,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="5" max="5" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2398,10 +2362,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2412,13 +2376,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F658B4C-7DBB-4EDF-981E-97E4B7C1F375}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
@@ -2448,7 +2412,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2459,13 +2423,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C921207-0810-405F-8F16-4133FFE6EA23}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -2473,8 +2437,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="68.1796875" collapsed="true"/>
+    <col min="5" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="68.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2491,7 +2455,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>42</v>
@@ -2500,12 +2464,12 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="1" ht="52" r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2518,24 +2482,24 @@
         <v>43</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row ht="29" r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2543,19 +2507,19 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>